<commit_message>
Fac allocation basic complete code
</commit_message>
<xml_diff>
--- a/fac_pref.xlsx
+++ b/fac_pref.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="50">
   <si>
     <t>facID</t>
   </si>
@@ -28,12 +29,6 @@
   </si>
   <si>
     <t>exp</t>
-  </si>
-  <si>
-    <t>pr1 exp</t>
-  </si>
-  <si>
-    <t>pr2 exp</t>
   </si>
   <si>
     <t>fac1</t>
@@ -163,6 +158,15 @@
   </si>
   <si>
     <t>410252D</t>
+  </si>
+  <si>
+    <t>pref_no</t>
+  </si>
+  <si>
+    <t>pr2_exp</t>
+  </si>
+  <si>
+    <t>pr1_exp</t>
   </si>
 </sst>
 </file>
@@ -501,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F217"/>
+  <dimension ref="A1:G217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F217"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +516,7 @@
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -526,18 +530,21 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <v>410250</v>
@@ -551,16 +558,19 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -571,13 +581,16 @@
       <c r="F3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4">
         <v>310251</v>
@@ -591,13 +604,16 @@
       <c r="F4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5">
         <v>310253</v>
@@ -611,13 +627,16 @@
       <c r="F5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>210251</v>
@@ -631,13 +650,16 @@
       <c r="F6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <v>210253</v>
@@ -651,16 +673,19 @@
       <c r="F7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -671,16 +696,19 @@
       <c r="F8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -691,13 +719,16 @@
       <c r="F9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10">
         <v>310253</v>
@@ -711,13 +742,16 @@
       <c r="F10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11">
         <v>310254</v>
@@ -731,13 +765,16 @@
       <c r="F11">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12">
         <v>210254</v>
@@ -751,13 +788,16 @@
       <c r="F12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13">
         <v>210251</v>
@@ -771,16 +811,19 @@
       <c r="F13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -791,13 +834,16 @@
       <c r="F14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15">
         <v>410251</v>
@@ -811,13 +857,16 @@
       <c r="F15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16">
         <v>310254</v>
@@ -831,13 +880,16 @@
       <c r="F16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17">
         <v>310253</v>
@@ -851,13 +903,16 @@
       <c r="F17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>210251</v>
@@ -871,13 +926,16 @@
       <c r="F18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C19">
         <v>210254</v>
@@ -891,13 +949,16 @@
       <c r="F19">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20">
         <v>410251</v>
@@ -911,16 +972,19 @@
       <c r="F20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21">
         <v>6</v>
@@ -931,13 +995,16 @@
       <c r="F21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22">
         <v>310254</v>
@@ -951,13 +1018,16 @@
       <c r="F22">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23">
         <v>310250</v>
@@ -971,13 +1041,16 @@
       <c r="F23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C24">
         <v>210251</v>
@@ -991,13 +1064,16 @@
       <c r="F24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25">
         <v>210254</v>
@@ -1011,16 +1087,19 @@
       <c r="F25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -1031,16 +1110,19 @@
       <c r="F26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D27">
         <v>2</v>
@@ -1051,13 +1133,16 @@
       <c r="F27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C28">
         <v>310250</v>
@@ -1071,13 +1156,16 @@
       <c r="F28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C29">
         <v>310253</v>
@@ -1091,13 +1179,16 @@
       <c r="F29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C30">
         <v>210251</v>
@@ -1111,13 +1202,16 @@
       <c r="F30">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C31">
         <v>210254</v>
@@ -1131,16 +1225,19 @@
       <c r="F31">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D32">
         <v>7</v>
@@ -1151,16 +1248,19 @@
       <c r="F32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1171,13 +1271,16 @@
       <c r="F33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C34">
         <v>310254</v>
@@ -1191,13 +1294,16 @@
       <c r="F34">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C35">
         <v>310251</v>
@@ -1211,13 +1317,16 @@
       <c r="F35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C36">
         <v>210254</v>
@@ -1231,13 +1340,16 @@
       <c r="F36">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C37">
         <v>210253</v>
@@ -1251,13 +1363,16 @@
       <c r="F37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C38">
         <v>410250</v>
@@ -1271,16 +1386,19 @@
       <c r="F38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D39">
         <v>2</v>
@@ -1291,13 +1409,16 @@
       <c r="F39">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C40">
         <v>310254</v>
@@ -1311,13 +1432,16 @@
       <c r="F40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C41">
         <v>310250</v>
@@ -1331,13 +1455,16 @@
       <c r="F41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C42">
         <v>210254</v>
@@ -1351,13 +1478,16 @@
       <c r="F42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C43">
         <v>210253</v>
@@ -1371,13 +1501,16 @@
       <c r="F43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C44">
         <v>410251</v>
@@ -1391,13 +1524,16 @@
       <c r="F44">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C45">
         <v>410250</v>
@@ -1411,13 +1547,16 @@
       <c r="F45">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C46">
         <v>310251</v>
@@ -1431,13 +1570,16 @@
       <c r="F46">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C47">
         <v>310250</v>
@@ -1451,13 +1593,16 @@
       <c r="F47">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C48">
         <v>210253</v>
@@ -1471,13 +1616,16 @@
       <c r="F48">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C49">
         <v>210251</v>
@@ -1491,37 +1639,43 @@
       <c r="F49">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C50" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <v>6</v>
+      </c>
+      <c r="G50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" t="s">
         <v>46</v>
       </c>
-      <c r="D50">
-        <v>3</v>
-      </c>
-      <c r="E50">
-        <v>4</v>
-      </c>
-      <c r="F50">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" t="s">
-        <v>42</v>
-      </c>
-      <c r="C51" t="s">
-        <v>48</v>
-      </c>
       <c r="D51">
         <v>6</v>
       </c>
@@ -1531,13 +1685,16 @@
       <c r="F51">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C52">
         <v>310253</v>
@@ -1551,13 +1708,16 @@
       <c r="F52">
         <v>8</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C53">
         <v>310250</v>
@@ -1571,13 +1731,16 @@
       <c r="F53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C54">
         <v>210253</v>
@@ -1591,13 +1754,16 @@
       <c r="F54">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C55">
         <v>210251</v>
@@ -1611,16 +1777,19 @@
       <c r="F55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B56" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C56" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D56">
         <v>8</v>
@@ -1631,13 +1800,16 @@
       <c r="F56">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B57" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C57">
         <v>410251</v>
@@ -1651,13 +1823,16 @@
       <c r="F57">
         <v>7</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B58" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C58">
         <v>310251</v>
@@ -1671,13 +1846,16 @@
       <c r="F58">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C59">
         <v>310250</v>
@@ -1691,13 +1869,16 @@
       <c r="F59">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B60" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C60">
         <v>210254</v>
@@ -1711,13 +1892,16 @@
       <c r="F60">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B61" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C61">
         <v>210253</v>
@@ -1731,13 +1915,16 @@
       <c r="F61">
         <v>7</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B62" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C62">
         <v>410251</v>
@@ -1751,13 +1938,16 @@
       <c r="F62">
         <v>7</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B63" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C63">
         <v>410250</v>
@@ -1771,13 +1961,16 @@
       <c r="F63">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C64">
         <v>310250</v>
@@ -1791,13 +1984,16 @@
       <c r="F64">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C65">
         <v>310253</v>
@@ -1811,13 +2007,16 @@
       <c r="F65">
         <v>8</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B66" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C66">
         <v>210254</v>
@@ -1831,13 +2030,16 @@
       <c r="F66">
         <v>6</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B67" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C67">
         <v>210251</v>
@@ -1851,13 +2053,16 @@
       <c r="F67">
         <v>8</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B68" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C68">
         <v>410251</v>
@@ -1871,16 +2076,19 @@
       <c r="F68">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B69" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C69" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D69">
         <v>4</v>
@@ -1891,13 +2099,16 @@
       <c r="F69">
         <v>4</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B70" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C70">
         <v>310253</v>
@@ -1911,13 +2122,16 @@
       <c r="F70">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B71" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C71">
         <v>310251</v>
@@ -1931,13 +2145,16 @@
       <c r="F71">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G71">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B72" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C72">
         <v>210253</v>
@@ -1951,13 +2168,16 @@
       <c r="F72">
         <v>6</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B73" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C73">
         <v>210251</v>
@@ -1971,16 +2191,19 @@
       <c r="F73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B74" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C74" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -1991,16 +2214,19 @@
       <c r="F74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B75" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C75" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D75">
         <v>5</v>
@@ -2011,13 +2237,16 @@
       <c r="F75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B76" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C76">
         <v>310253</v>
@@ -2031,13 +2260,16 @@
       <c r="F76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B77" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C77">
         <v>310250</v>
@@ -2051,13 +2283,16 @@
       <c r="F77">
         <v>6</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B78" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C78">
         <v>210251</v>
@@ -2071,13 +2306,16 @@
       <c r="F78">
         <v>8</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B79" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C79">
         <v>210254</v>
@@ -2091,13 +2329,16 @@
       <c r="F79">
         <v>7</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B80" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C80">
         <v>410251</v>
@@ -2111,16 +2352,19 @@
       <c r="F80">
         <v>8</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C81" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D81">
         <v>2</v>
@@ -2131,13 +2375,16 @@
       <c r="F81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B82" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C82">
         <v>310251</v>
@@ -2151,13 +2398,16 @@
       <c r="F82">
         <v>8</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C83">
         <v>310254</v>
@@ -2171,13 +2421,16 @@
       <c r="F83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B84" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C84">
         <v>210254</v>
@@ -2191,13 +2444,16 @@
       <c r="F84">
         <v>3</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G84">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C85">
         <v>210253</v>
@@ -2211,16 +2467,19 @@
       <c r="F85">
         <v>4</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B86" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C86" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -2231,16 +2490,19 @@
       <c r="F86">
         <v>5</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G86">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B87" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C87" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -2251,13 +2513,16 @@
       <c r="F87">
         <v>6</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B88" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C88">
         <v>310251</v>
@@ -2271,13 +2536,16 @@
       <c r="F88">
         <v>4</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B89" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C89">
         <v>310250</v>
@@ -2291,13 +2559,16 @@
       <c r="F89">
         <v>3</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B90" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C90">
         <v>210254</v>
@@ -2311,13 +2582,16 @@
       <c r="F90">
         <v>2</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B91" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C91">
         <v>210253</v>
@@ -2331,13 +2605,16 @@
       <c r="F91">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G91">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B92" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C92">
         <v>410251</v>
@@ -2351,16 +2628,19 @@
       <c r="F92">
         <v>2</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B93" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C93" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D93">
         <v>6</v>
@@ -2371,13 +2651,16 @@
       <c r="F93">
         <v>8</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G93">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B94" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C94">
         <v>310251</v>
@@ -2391,13 +2674,16 @@
       <c r="F94">
         <v>6</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G94">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B95" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C95">
         <v>310254</v>
@@ -2411,13 +2697,16 @@
       <c r="F95">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G95">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B96" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C96">
         <v>210254</v>
@@ -2431,13 +2720,16 @@
       <c r="F96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B97" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C97">
         <v>210251</v>
@@ -2451,16 +2743,19 @@
       <c r="F97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G97">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B98" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C98" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D98">
         <v>8</v>
@@ -2471,13 +2766,16 @@
       <c r="F98">
         <v>7</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B99" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C99">
         <v>410251</v>
@@ -2491,13 +2789,16 @@
       <c r="F99">
         <v>2</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B100" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C100">
         <v>310251</v>
@@ -2511,13 +2812,16 @@
       <c r="F100">
         <v>6</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B101" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C101">
         <v>310254</v>
@@ -2531,13 +2835,16 @@
       <c r="F101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G101">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B102" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C102">
         <v>210251</v>
@@ -2551,13 +2858,16 @@
       <c r="F102">
         <v>3</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G102">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B103" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C103">
         <v>210253</v>
@@ -2571,16 +2881,19 @@
       <c r="F103">
         <v>3</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B104" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C104" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D104">
         <v>7</v>
@@ -2591,13 +2904,16 @@
       <c r="F104">
         <v>3</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B105" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C105">
         <v>410250</v>
@@ -2611,13 +2927,16 @@
       <c r="F105">
         <v>2</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B106" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C106">
         <v>310250</v>
@@ -2631,13 +2950,16 @@
       <c r="F106">
         <v>8</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G106">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B107" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C107">
         <v>310251</v>
@@ -2651,13 +2973,16 @@
       <c r="F107">
         <v>7</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G107">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B108" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C108">
         <v>210251</v>
@@ -2671,13 +2996,16 @@
       <c r="F108">
         <v>7</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G108">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B109" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C109">
         <v>210253</v>
@@ -2691,16 +3019,19 @@
       <c r="F109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G109">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B110" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C110" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D110">
         <v>5</v>
@@ -2711,13 +3042,16 @@
       <c r="F110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G110">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B111" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C111">
         <v>410251</v>
@@ -2731,13 +3065,16 @@
       <c r="F111">
         <v>5</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G111">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B112" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C112">
         <v>310250</v>
@@ -2751,13 +3088,16 @@
       <c r="F112">
         <v>8</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B113" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C113">
         <v>310253</v>
@@ -2771,13 +3111,16 @@
       <c r="F113">
         <v>4</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G113">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B114" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C114">
         <v>210251</v>
@@ -2791,13 +3134,16 @@
       <c r="F114">
         <v>5</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G114">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B115" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C115">
         <v>210253</v>
@@ -2811,13 +3157,16 @@
       <c r="F115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B116" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C116">
         <v>410251</v>
@@ -2831,13 +3180,16 @@
       <c r="F116">
         <v>8</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B117" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C117">
         <v>410250</v>
@@ -2851,13 +3203,16 @@
       <c r="F117">
         <v>6</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B118" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C118">
         <v>310253</v>
@@ -2871,13 +3226,16 @@
       <c r="F118">
         <v>4</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B119" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C119">
         <v>310251</v>
@@ -2891,13 +3249,16 @@
       <c r="F119">
         <v>2</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G119">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B120" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C120">
         <v>210254</v>
@@ -2911,13 +3272,16 @@
       <c r="F120">
         <v>4</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G120">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B121" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C121">
         <v>210251</v>
@@ -2931,16 +3295,19 @@
       <c r="F121">
         <v>3</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G121">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B122" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C122" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D122">
         <v>5</v>
@@ -2951,16 +3318,19 @@
       <c r="F122">
         <v>4</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B123" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C123" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D123">
         <v>8</v>
@@ -2971,13 +3341,16 @@
       <c r="F123">
         <v>2</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G123">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B124" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C124">
         <v>310251</v>
@@ -2991,13 +3364,16 @@
       <c r="F124">
         <v>6</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B125" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C125">
         <v>310250</v>
@@ -3011,13 +3387,16 @@
       <c r="F125">
         <v>3</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G125">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B126" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C126">
         <v>210254</v>
@@ -3031,13 +3410,16 @@
       <c r="F126">
         <v>7</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G126">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B127" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C127">
         <v>210253</v>
@@ -3051,13 +3433,16 @@
       <c r="F127">
         <v>8</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B128" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C128">
         <v>410250</v>
@@ -3071,13 +3456,16 @@
       <c r="F128">
         <v>8</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B129" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C129">
         <v>410251</v>
@@ -3091,13 +3479,16 @@
       <c r="F129">
         <v>4</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G129">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B130" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C130">
         <v>310253</v>
@@ -3111,13 +3502,16 @@
       <c r="F130">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G130">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B131" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C131">
         <v>310254</v>
@@ -3131,13 +3525,16 @@
       <c r="F131">
         <v>7</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G131">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B132" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C132">
         <v>210254</v>
@@ -3151,13 +3548,16 @@
       <c r="F132">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B133" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C133">
         <v>210251</v>
@@ -3171,13 +3571,16 @@
       <c r="F133">
         <v>8</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G133">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B134" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C134">
         <v>410251</v>
@@ -3191,16 +3594,19 @@
       <c r="F134">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B135" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C135" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D135">
         <v>3</v>
@@ -3211,13 +3617,16 @@
       <c r="F135">
         <v>2</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G135">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B136" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C136">
         <v>310253</v>
@@ -3231,13 +3640,16 @@
       <c r="F136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B137" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C137">
         <v>310254</v>
@@ -3251,13 +3663,16 @@
       <c r="F137">
         <v>2</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G137">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B138" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C138">
         <v>210254</v>
@@ -3271,13 +3686,16 @@
       <c r="F138">
         <v>8</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G138">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B139" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C139">
         <v>210251</v>
@@ -3291,16 +3709,19 @@
       <c r="F139">
         <v>4</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G139">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B140" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C140" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D140">
         <v>2</v>
@@ -3311,16 +3732,19 @@
       <c r="F140">
         <v>2</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B141" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C141" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D141">
         <v>3</v>
@@ -3331,13 +3755,16 @@
       <c r="F141">
         <v>3</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B142" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C142">
         <v>310251</v>
@@ -3351,13 +3778,16 @@
       <c r="F142">
         <v>2</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G142">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B143" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C143">
         <v>310253</v>
@@ -3371,13 +3801,16 @@
       <c r="F143">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G143">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B144" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C144">
         <v>210253</v>
@@ -3391,13 +3824,16 @@
       <c r="F144">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G144">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B145" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C145">
         <v>210254</v>
@@ -3411,13 +3847,16 @@
       <c r="F145">
         <v>8</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G145">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B146" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C146">
         <v>410250</v>
@@ -3431,16 +3870,19 @@
       <c r="F146">
         <v>2</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G146">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B147" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C147" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D147">
         <v>7</v>
@@ -3451,13 +3893,16 @@
       <c r="F147">
         <v>3</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G147">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B148" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C148">
         <v>310250</v>
@@ -3471,13 +3916,16 @@
       <c r="F148">
         <v>4</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G148">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B149" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C149">
         <v>310254</v>
@@ -3491,13 +3939,16 @@
       <c r="F149">
         <v>5</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B150" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C150">
         <v>210251</v>
@@ -3511,13 +3962,16 @@
       <c r="F150">
         <v>3</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G150">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B151" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C151">
         <v>210253</v>
@@ -3531,16 +3985,19 @@
       <c r="F151">
         <v>3</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B152" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C152" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D152">
         <v>3</v>
@@ -3551,13 +4008,16 @@
       <c r="F152">
         <v>8</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G152">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B153" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C153">
         <v>410250</v>
@@ -3571,13 +4031,16 @@
       <c r="F153">
         <v>7</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G153">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B154" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C154">
         <v>310254</v>
@@ -3591,13 +4054,16 @@
       <c r="F154">
         <v>5</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G154">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B155" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C155">
         <v>310251</v>
@@ -3611,13 +4077,16 @@
       <c r="F155">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B156" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C156">
         <v>210253</v>
@@ -3631,13 +4100,16 @@
       <c r="F156">
         <v>2</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G156">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B157" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C157">
         <v>210251</v>
@@ -3651,16 +4123,19 @@
       <c r="F157">
         <v>1</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G157">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B158" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C158" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D158">
         <v>8</v>
@@ -3671,16 +4146,19 @@
       <c r="F158">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G158">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B159" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C159" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D159">
         <v>1</v>
@@ -3691,13 +4169,16 @@
       <c r="F159">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G159">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B160" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C160">
         <v>310250</v>
@@ -3711,13 +4192,16 @@
       <c r="F160">
         <v>4</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G160">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B161" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C161">
         <v>310253</v>
@@ -3731,13 +4215,16 @@
       <c r="F161">
         <v>1</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G161">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B162" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C162">
         <v>210253</v>
@@ -3751,13 +4238,16 @@
       <c r="F162">
         <v>7</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B163" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C163">
         <v>210254</v>
@@ -3771,16 +4261,19 @@
       <c r="F163">
         <v>5</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B164" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C164" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D164">
         <v>5</v>
@@ -3791,16 +4284,19 @@
       <c r="F164">
         <v>8</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G164">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B165" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C165" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D165">
         <v>2</v>
@@ -3811,13 +4307,16 @@
       <c r="F165">
         <v>7</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B166" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C166">
         <v>310251</v>
@@ -3831,13 +4330,16 @@
       <c r="F166">
         <v>1</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G166">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B167" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C167">
         <v>310250</v>
@@ -3851,13 +4353,16 @@
       <c r="F167">
         <v>8</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G167">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B168" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C168">
         <v>210254</v>
@@ -3871,13 +4376,16 @@
       <c r="F168">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G168">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B169" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C169">
         <v>210253</v>
@@ -3891,13 +4399,16 @@
       <c r="F169">
         <v>3</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G169">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B170" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C170">
         <v>410251</v>
@@ -3911,13 +4422,16 @@
       <c r="F170">
         <v>5</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G170">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B171" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C171">
         <v>410250</v>
@@ -3931,13 +4445,16 @@
       <c r="F171">
         <v>1</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G171">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B172" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C172">
         <v>310250</v>
@@ -3951,13 +4468,16 @@
       <c r="F172">
         <v>7</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B173" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C173">
         <v>310253</v>
@@ -3971,13 +4491,16 @@
       <c r="F173">
         <v>2</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G173">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B174" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C174">
         <v>210254</v>
@@ -3991,13 +4514,16 @@
       <c r="F174">
         <v>2</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G174">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B175" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C175">
         <v>210251</v>
@@ -4011,13 +4537,16 @@
       <c r="F175">
         <v>1</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G175">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B176" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C176">
         <v>410250</v>
@@ -4031,16 +4560,19 @@
       <c r="F176">
         <v>6</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G176">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B177" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C177" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D177">
         <v>6</v>
@@ -4051,13 +4583,16 @@
       <c r="F177">
         <v>2</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G177">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B178" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C178">
         <v>310254</v>
@@ -4071,13 +4606,16 @@
       <c r="F178">
         <v>7</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G178">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B179" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C179">
         <v>310251</v>
@@ -4091,13 +4629,16 @@
       <c r="F179">
         <v>5</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G179">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B180" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C180">
         <v>210251</v>
@@ -4111,13 +4652,16 @@
       <c r="F180">
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B181" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C181">
         <v>210254</v>
@@ -4131,13 +4675,16 @@
       <c r="F181">
         <v>6</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G181">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B182" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C182">
         <v>410251</v>
@@ -4151,16 +4698,19 @@
       <c r="F182">
         <v>3</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G182">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B183" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C183" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D183">
         <v>1</v>
@@ -4171,13 +4721,16 @@
       <c r="F183">
         <v>4</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G183">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B184" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C184">
         <v>310254</v>
@@ -4191,13 +4744,16 @@
       <c r="F184">
         <v>1</v>
       </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G184">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B185" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C185">
         <v>310250</v>
@@ -4211,13 +4767,16 @@
       <c r="F185">
         <v>7</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G185">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B186" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C186">
         <v>210251</v>
@@ -4231,13 +4790,16 @@
       <c r="F186">
         <v>6</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G186">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B187" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C187">
         <v>210254</v>
@@ -4251,13 +4813,16 @@
       <c r="F187">
         <v>2</v>
       </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B188" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C188">
         <v>410251</v>
@@ -4271,16 +4836,19 @@
       <c r="F188">
         <v>8</v>
       </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G188">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B189" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C189" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D189">
         <v>8</v>
@@ -4291,13 +4859,16 @@
       <c r="F189">
         <v>7</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G189">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B190" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C190">
         <v>310250</v>
@@ -4311,13 +4882,16 @@
       <c r="F190">
         <v>3</v>
       </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B191" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C191">
         <v>310251</v>
@@ -4331,13 +4905,16 @@
       <c r="F191">
         <v>3</v>
       </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G191">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B192" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C192">
         <v>210251</v>
@@ -4351,13 +4928,16 @@
       <c r="F192">
         <v>1</v>
       </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G192">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B193" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C193">
         <v>210253</v>
@@ -4371,37 +4951,43 @@
       <c r="F193">
         <v>8</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G193">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B194" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C194" t="s">
+        <v>44</v>
+      </c>
+      <c r="D194">
+        <v>3</v>
+      </c>
+      <c r="E194">
+        <v>6</v>
+      </c>
+      <c r="F194">
+        <v>5</v>
+      </c>
+      <c r="G194">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>36</v>
+      </c>
+      <c r="B195" t="s">
+        <v>40</v>
+      </c>
+      <c r="C195" t="s">
         <v>46</v>
       </c>
-      <c r="D194">
-        <v>3</v>
-      </c>
-      <c r="E194">
-        <v>6</v>
-      </c>
-      <c r="F194">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>38</v>
-      </c>
-      <c r="B195" t="s">
-        <v>42</v>
-      </c>
-      <c r="C195" t="s">
-        <v>48</v>
-      </c>
       <c r="D195">
         <v>4</v>
       </c>
@@ -4411,13 +4997,16 @@
       <c r="F195">
         <v>2</v>
       </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G195">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B196" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C196">
         <v>310254</v>
@@ -4431,13 +5020,16 @@
       <c r="F196">
         <v>6</v>
       </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G196">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B197" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C197">
         <v>310250</v>
@@ -4451,13 +5043,16 @@
       <c r="F197">
         <v>1</v>
       </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B198" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C198">
         <v>210253</v>
@@ -4471,13 +5066,16 @@
       <c r="F198">
         <v>0</v>
       </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G198">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B199" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C199">
         <v>210254</v>
@@ -4491,16 +5089,19 @@
       <c r="F199">
         <v>3</v>
       </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G199">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B200" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C200" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D200">
         <v>7</v>
@@ -4511,13 +5112,16 @@
       <c r="F200">
         <v>1</v>
       </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G200">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B201" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C201">
         <v>410251</v>
@@ -4531,13 +5135,16 @@
       <c r="F201">
         <v>5</v>
       </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G201">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B202" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C202">
         <v>310250</v>
@@ -4551,13 +5158,16 @@
       <c r="F202">
         <v>7</v>
       </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G202">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B203" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C203">
         <v>310251</v>
@@ -4571,13 +5181,16 @@
       <c r="F203">
         <v>0</v>
       </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B204" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C204">
         <v>210251</v>
@@ -4591,13 +5204,16 @@
       <c r="F204">
         <v>1</v>
       </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G204">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B205" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C205">
         <v>210254</v>
@@ -4611,13 +5227,16 @@
       <c r="F205">
         <v>3</v>
       </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G205">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B206" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C206">
         <v>410250</v>
@@ -4631,16 +5250,19 @@
       <c r="F206">
         <v>5</v>
       </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G206">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B207" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C207" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D207">
         <v>7</v>
@@ -4651,13 +5273,16 @@
       <c r="F207">
         <v>8</v>
       </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G207">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B208" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C208">
         <v>310250</v>
@@ -4671,13 +5296,16 @@
       <c r="F208">
         <v>1</v>
       </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G208">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B209" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C209">
         <v>310251</v>
@@ -4691,13 +5319,16 @@
       <c r="F209">
         <v>4</v>
       </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G209">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B210" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C210">
         <v>210254</v>
@@ -4711,13 +5342,16 @@
       <c r="F210">
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G210">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B211" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C211">
         <v>210251</v>
@@ -4731,37 +5365,43 @@
       <c r="F211">
         <v>3</v>
       </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B212" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C212" t="s">
+        <v>43</v>
+      </c>
+      <c r="D212">
+        <v>4</v>
+      </c>
+      <c r="E212">
+        <v>3</v>
+      </c>
+      <c r="F212">
+        <v>7</v>
+      </c>
+      <c r="G212">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>39</v>
+      </c>
+      <c r="B213" t="s">
+        <v>40</v>
+      </c>
+      <c r="C213" t="s">
         <v>45</v>
       </c>
-      <c r="D212">
-        <v>4</v>
-      </c>
-      <c r="E212">
-        <v>3</v>
-      </c>
-      <c r="F212">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
-        <v>41</v>
-      </c>
-      <c r="B213" t="s">
-        <v>42</v>
-      </c>
-      <c r="C213" t="s">
-        <v>47</v>
-      </c>
       <c r="D213">
         <v>7</v>
       </c>
@@ -4771,13 +5411,16 @@
       <c r="F213">
         <v>8</v>
       </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B214" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C214">
         <v>310254</v>
@@ -4791,13 +5434,16 @@
       <c r="F214">
         <v>3</v>
       </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G214">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B215" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C215">
         <v>310253</v>
@@ -4811,13 +5457,16 @@
       <c r="F215">
         <v>2</v>
       </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G215">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B216" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C216">
         <v>210254</v>
@@ -4831,13 +5480,16 @@
       <c r="F216">
         <v>5</v>
       </c>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G216">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B217" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C217">
         <v>210253</v>
@@ -4850,6 +5502,9 @@
       </c>
       <c r="F217">
         <v>6</v>
+      </c>
+      <c r="G217">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>